<commit_message>
update figures for Greedy Caching
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="12450" activeTab="4"/>
+    <workbookView windowWidth="27720" windowHeight="12450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SA Hyper Tuning" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
     <t>0.9705    0.9657    0.6649    0.9682</t>
   </si>
   <si>
-    <t>757.9589    0.3022    0.0086    0.0039</t>
+    <t>757.9589    0.3022    0.0026    0.0039</t>
   </si>
   <si>
     <t>(P2)</t>
@@ -182,22 +182,22 @@
     <t>31.7881    0.2209    0.0023    0.0047</t>
   </si>
   <si>
-    <t>6.5510    4.6880    1.5188    4.6631</t>
-  </si>
-  <si>
-    <t>0.9806    0.9174    0.4840    0.9624</t>
+    <t>6.5510    4.6880    1.6008    4.4724</t>
+  </si>
+  <si>
+    <t>0.9806    0.9174    0.5046    0.9600</t>
   </si>
   <si>
     <t>153.3777    0.2277    0.0029    0.0059</t>
   </si>
   <si>
-    <t>7.0654    4.5582    1.5133    4.4397</t>
-  </si>
-  <si>
-    <t>0.9801    0.9107    0.4720    0.9406</t>
-  </si>
-  <si>
-    <t>374.2171    0.3599    0.0086    0.0078</t>
+    <t>7.0654    4.5582    1.5114    4.2913</t>
+  </si>
+  <si>
+    <t>0.9801    0.9107    0.4594    0.9377</t>
+  </si>
+  <si>
+    <t>374.2171    0.3599    0.0086    0.0087</t>
   </si>
   <si>
     <t>6.9602    4.6854    1.4943    4.2896</t>
@@ -206,7 +206,7 @@
     <t>0.9604    0.8927    0.4583    0.9061</t>
   </si>
   <si>
-    <t>709.4593    0.3842    0.0095    0.0092</t>
+    <t>709.4593    0.3842    0.0095    0.0095</t>
   </si>
   <si>
     <t>100 Users</t>
@@ -239,7 +239,7 @@
     <t>4.4495    4.1445    2.6825    2.6060</t>
   </si>
   <si>
-    <t xml:space="preserve"> 4.7213    4.5881    3.6827    2.7222</t>
+    <t>4.7213    4.5881    3.6115    2.6855</t>
   </si>
   <si>
     <t>0.5GB</t>
@@ -251,7 +251,7 @@
     <t>4.6396    4.4532    2.8655    2.8760</t>
   </si>
   <si>
-    <t>4.7337    4.6157    3.8581    3.0928</t>
+    <t>4.7337    4.6157    3.6631    2.9180</t>
   </si>
   <si>
     <t>0.75GB</t>
@@ -266,7 +266,7 @@
     <t>4.6140    4.4198    2.8722    2.9662</t>
   </si>
   <si>
-    <t>4.7269    4.5977    3.4637    2.7796</t>
+    <t>4.7269    4.5977    3.6678    2.9588</t>
   </si>
   <si>
     <t>1GB</t>
@@ -281,7 +281,7 @@
     <t>4.6842    4.5402    3.0278    3.0740</t>
   </si>
   <si>
-    <t xml:space="preserve"> 4.7222    4.6207    3.2578    2.7004</t>
+    <t>4.7222    4.6207    3.6525    2.9961</t>
   </si>
   <si>
     <t>Cache-Hit Ratio (P1)</t>
@@ -305,7 +305,7 @@
     <t>1.0000    1.0000    0.8759    1.0000</t>
   </si>
   <si>
-    <t>1.0000    1.0000    0.9742    1.0000</t>
+    <t>1.0000    1.0000    0.9542    1.0000</t>
   </si>
   <si>
     <t>0.9957    0.9943    0.5337    0.9955</t>
@@ -317,7 +317,7 @@
     <t>1.0000    1.0000    0.8688    1.0000</t>
   </si>
   <si>
-    <t>1.0000    1.0000    0.9341    1.0000</t>
+    <t>1.0000    1.0000    0.9548    1.0000</t>
   </si>
   <si>
     <t>1.0000    1.0000    0.5154    1.0000</t>
@@ -329,7 +329,7 @@
     <t>1.0000    1.0000    0.8815    1.0000</t>
   </si>
   <si>
-    <t>1.0000    1.0000    0.9125    1.0000</t>
+    <t>1.0000    1.0000    0.9531    1.0000</t>
   </si>
   <si>
     <t>Energy Gain (P2)</t>
@@ -368,8 +368,7 @@
     <t>6.9549    6.6557    2.4896    5.1621</t>
   </si>
   <si>
-    <t xml:space="preserve">6.1004    5.4621    1.2844    5.2472
-</t>
+    <t>6.1004    5.4621    1.2844    5.2472</t>
   </si>
   <si>
     <t>6.6124    5.9671    1.7730    5.3193</t>
@@ -681,8 +680,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -715,21 +714,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -746,7 +738,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -754,14 +746,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -777,15 +808,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -799,40 +822,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -859,7 +858,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -871,13 +918,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -889,19 +984,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -913,121 +1026,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1038,41 +1037,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1096,6 +1060,50 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1129,162 +1137,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2223,7 +2222,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -2519,8 +2518,8 @@
   <sheetPr/>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -2937,8 +2936,8 @@
   <sheetPr/>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15.75" outlineLevelCol="6"/>
@@ -3302,8 +3301,8 @@
   <sheetPr/>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15.75" outlineLevelCol="6"/>

</xml_diff>